<commit_message>
Updated labels in excel sheet
</commit_message>
<xml_diff>
--- a/R_code/Empty_autosalt_form.xlsx
+++ b/R_code/Empty_autosalt_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margo.DESKTOP-T66VM01\Desktop\VIU\Salt_Dilution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margo.DESKTOP-T66VM01\Desktop\VIU\GitHub\R_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3905D3F-548E-490A-B09D-D85D842DC05F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B29D3E3-9026-4979-A42F-B01EAC78604A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EC salt waves" sheetId="13" r:id="rId1"/>
@@ -66,12 +66,6 @@
   </si>
   <si>
     <t>Ecb</t>
-  </si>
-  <si>
-    <t>ECb start</t>
-  </si>
-  <si>
-    <t>ECb end</t>
   </si>
   <si>
     <t>Date and time</t>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>Stage [cm]</t>
+  </si>
+  <si>
+    <t>Wave start</t>
+  </si>
+  <si>
+    <t>Wave end</t>
   </si>
 </sst>
 </file>
@@ -346,10 +346,10 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +477,7 @@
           <c:idx val="2"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>ECb1</c:v>
+            <c:v>EC1_wave</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -530,7 +530,7 @@
           <c:idx val="4"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>ECb2</c:v>
+            <c:v>EC2_wave</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -583,7 +583,7 @@
           <c:idx val="8"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>ECb3</c:v>
+            <c:v>EC3_wave</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -638,7 +638,7 @@
           <c:idx val="3"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>ECb4</c:v>
+            <c:v>EC4_wave</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -3013,8 +3013,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X2701"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3023,7 +3023,9 @@
     <col min="3" max="3" width="10.26953125" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="10" width="10.1796875" style="18" customWidth="1"/>
     <col min="11" max="11" width="10.1796875" style="13" customWidth="1"/>
-    <col min="12" max="16" width="9.1796875" style="13"/>
+    <col min="12" max="12" width="9.1796875" style="13"/>
+    <col min="13" max="13" width="10.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.1796875" style="13"/>
     <col min="17" max="17" width="14.08984375" style="13" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="9.1796875" style="13"/>
     <col min="21" max="21" width="15.453125" style="13" customWidth="1"/>
@@ -3049,7 +3051,7 @@
     </row>
     <row r="2" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="13"/>
@@ -3076,55 +3078,55 @@
     <row r="4" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
-      <c r="M4" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="Q4" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
+      <c r="M4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="Q4" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
     </row>
     <row r="5" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>22</v>
       </c>
       <c r="L5" s="20"/>
       <c r="M5" s="21"/>
@@ -3154,12 +3156,12 @@
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="M6" s="16" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="N6" s="25"/>
       <c r="O6" s="28"/>
       <c r="Q6" s="16" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="28"/>
@@ -3176,12 +3178,12 @@
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="M7" s="16" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="N7" s="25"/>
       <c r="O7" s="28"/>
       <c r="Q7" s="16" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="R7" s="25"/>
       <c r="S7" s="28"/>
@@ -3198,17 +3200,17 @@
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="M8" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N8" s="25"/>
       <c r="O8" s="28"/>
       <c r="Q8" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="28"/>
       <c r="U8" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="V8" s="17"/>
       <c r="W8" s="16" t="s">
@@ -3228,7 +3230,7 @@
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="U9" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="V9" s="17"/>
       <c r="W9" s="16" t="s">
@@ -3260,7 +3262,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="V10" s="17"/>
       <c r="W10" s="16" t="s">
@@ -3291,18 +3293,18 @@
         <f t="shared" ref="J11:J74" si="3">AVERAGE(F7:F15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="Q11" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
+      <c r="M11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="Q11" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
       <c r="U11" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="V11" s="17"/>
       <c r="W11" s="16" t="s">
@@ -3372,12 +3374,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="28"/>
       <c r="Q13" s="16" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="R13" s="25"/>
       <c r="S13" s="28"/>
@@ -3406,12 +3408,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="28"/>
       <c r="Q14" s="16" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="R14" s="25"/>
       <c r="S14" s="28"/>
@@ -3440,12 +3442,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="28"/>
       <c r="Q15" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R15" s="25"/>
       <c r="S15" s="28"/>
@@ -67929,7 +67931,7 @@
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="G10:J2701" evalError="1"/>
+    <ignoredError sqref="G11:J2701 H10:J10" evalError="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -67965,7 +67967,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.3">
@@ -67973,16 +67975,16 @@
     </row>
     <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -68012,7 +68014,7 @@
       <c r="C7" s="26"/>
       <c r="D7" s="8"/>
       <c r="G7" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H7" s="10" t="e">
         <f>(AVERAGEIFS(D5:D544,A5:A544,"yes"))</f>
@@ -68028,7 +68030,7 @@
       <c r="C8" s="26"/>
       <c r="D8" s="8"/>
       <c r="G8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H8" s="11" t="e" cm="1">
         <f t="array" ref="H8">(_xlfn.STDEV.P(IF($A$5:$A$544="yes",$D$5:$D$544)))</f>
@@ -68044,7 +68046,7 @@
       <c r="C9" s="26"/>
       <c r="D9" s="8"/>
       <c r="G9" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" s="11" cm="1">
         <f t="array" ref="H9">(MAX(IF($A$5:$A$544="yes",$D$5:$D$544)))</f>
@@ -68060,7 +68062,7 @@
       <c r="C10" s="26"/>
       <c r="D10" s="8"/>
       <c r="G10" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H10" s="11" cm="1">
         <f t="array" ref="H10">(MIN(IF($A$5:$A$544="yes",$D$5:$D$544)))</f>

</xml_diff>